<commit_message>
added some mixture variation-related files to chem/
</commit_message>
<xml_diff>
--- a/chem/varmix.xlsx
+++ b/chem/varmix.xlsx
@@ -446,17 +446,17 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>CN-0.45</t>
+          <t>CN-0.48</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>CN-0.30</t>
+          <t>CN-0.32</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>CN-0.15</t>
+          <t>CN-0.16</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -493,13 +493,13 @@
         <v>0.732597680268234</v>
       </c>
       <c r="D2" t="n">
-        <v>0.7347135247630321</v>
+        <v>0.7346787552966266</v>
       </c>
       <c r="E2" t="n">
-        <v>0.7348309150611853</v>
+        <v>0.7348204868701099</v>
       </c>
       <c r="F2" t="n">
-        <v>0.7348599715223593</v>
+        <v>0.7348607179829629</v>
       </c>
       <c r="G2" t="n">
         <v>0.7348016213614881</v>
@@ -527,13 +527,13 @@
         <v>0.247626307635559</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2483414870224034</v>
+        <v>0.2483297345492298</v>
       </c>
       <c r="E3" t="n">
-        <v>0.2483811662718289</v>
+        <v>0.2483776414252169</v>
       </c>
       <c r="F3" t="n">
-        <v>0.2483909876845733</v>
+        <v>0.248391239996706</v>
       </c>
       <c r="G3" t="n">
         <v>0.2483712646697787</v>
@@ -561,13 +561,13 @@
         <v>0.01977601209620681</v>
       </c>
       <c r="D4" t="n">
-        <v>0.01694498821456444</v>
+        <v>0.01699151015414339</v>
       </c>
       <c r="E4" t="n">
-        <v>0.01678791866698569</v>
+        <v>0.01680187170467322</v>
       </c>
       <c r="F4" t="n">
-        <v>0.01674904079306725</v>
+        <v>0.01674804202033104</v>
       </c>
       <c r="G4" t="n">
         <v>0.01682711396873312</v>
@@ -595,13 +595,13 @@
         <v>0.02699436898157527</v>
       </c>
       <c r="D5" t="n">
-        <v>0.02306339497429249</v>
+        <v>0.0231278093066446</v>
       </c>
       <c r="E5" t="n">
-        <v>0.02284596132647448</v>
+        <v>0.02286527390688169</v>
       </c>
       <c r="F5" t="n">
-        <v>0.02279215284834389</v>
+        <v>0.02279077056438785</v>
       </c>
       <c r="G5" t="n">
         <v>0.02290021344475908</v>
@@ -629,13 +629,13 @@
         <v>0.9995792123477809</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9995074924069265</v>
+        <v>0.9995088641126235</v>
       </c>
       <c r="E6" t="n">
-        <v>0.9995028050260363</v>
+        <v>0.9995032249693071</v>
       </c>
       <c r="F6" t="n">
-        <v>0.9995016312314825</v>
+        <v>0.9995016010048979</v>
       </c>
       <c r="G6" t="n">
         <v>0.999503982913771</v>
@@ -833,13 +833,13 @@
         <v>8.52</v>
       </c>
       <c r="D12" t="n">
-        <v>8.55283</v>
+        <v>8.559533199999999</v>
       </c>
       <c r="E12" t="n">
-        <v>8.52655</v>
+        <v>8.5293572</v>
       </c>
       <c r="F12" t="n">
-        <v>8.51233</v>
+        <v>8.512902799999999</v>
       </c>
       <c r="G12" t="n">
         <v>8.51017</v>
@@ -867,13 +867,13 @@
         <v>7.92</v>
       </c>
       <c r="D13" t="n">
-        <v>7.8536825</v>
+        <v>7.8528992</v>
       </c>
       <c r="E13" t="n">
-        <v>7.867669999999999</v>
+        <v>7.8648352</v>
       </c>
       <c r="F13" t="n">
-        <v>7.8984425</v>
+        <v>7.8958688</v>
       </c>
       <c r="G13" t="n">
         <v>7.946</v>

</xml_diff>